<commit_message>
Read receipt entry Excel
</commit_message>
<xml_diff>
--- a/ReceiptEntryTemplate.xlsx
+++ b/ReceiptEntryTemplate.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElixirAutomation\Demo Vedios &amp; Document\Receipt &amp; payment entry concept\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\readMultipleExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B97286A-75CB-4D53-BB16-B920D340B098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395F1460-C8C4-46B5-9501-F6FC4CBEDC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Receipt" sheetId="2" r:id="rId1"/>
@@ -187,9 +187,6 @@
     <t>CC Unique</t>
   </si>
   <si>
-    <t>Rp unique</t>
-  </si>
-  <si>
     <t>RE001</t>
   </si>
   <si>
@@ -275,6 +272,9 @@
   </si>
   <si>
     <t>RP007</t>
+  </si>
+  <si>
+    <t>RP unique</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FB9C7A-829F-4147-8F69-BE0A54978083}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -773,7 +775,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -811,7 +813,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -849,7 +851,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -887,7 +889,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -925,7 +927,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -963,7 +965,7 @@
     </row>
     <row r="7" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -1001,7 +1003,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -1039,7 +1041,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1077,7 +1079,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -1115,7 +1117,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -1154,6 +1156,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1162,7 +1165,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,10 +1194,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1205,10 +1208,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -1219,10 +1222,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -1233,10 +1236,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -1247,10 +1250,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -1261,10 +1264,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
@@ -1275,10 +1278,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1289,10 +1292,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -1303,10 +1306,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -1317,10 +1320,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>37</v>
@@ -1371,10 +1374,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
@@ -1388,10 +1391,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -1412,7 +1415,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B92B39-6115-4F83-A1E8-7596FD90A200}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1423,7 +1428,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>50</v>
@@ -1437,10 +1442,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1451,10 +1456,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>39</v>
@@ -1465,10 +1470,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
@@ -1479,10 +1484,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -1493,10 +1498,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -1507,10 +1512,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
@@ -1521,10 +1526,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
@@ -1536,5 +1541,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>